<commit_message>
more work on updating pintle post mortem
</commit_message>
<xml_diff>
--- a/analysis/Pintle_V1 testing/Pintle Test 01-19-2019/00 Pintle Data Analysis 01-19-2019.xlsx
+++ b/analysis/Pintle_V1 testing/Pintle Test 01-19-2019/00 Pintle Data Analysis 01-19-2019.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40471A4C-69F5-4092-AEF9-ABB25C8341B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD87B40-3357-4DD7-9150-9A3816B2F1CB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1020" windowWidth="8835" windowHeight="10725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1605" yWindow="540" windowWidth="16320" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Summary" sheetId="1" r:id="rId1"/>
@@ -2970,8 +2970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>